<commit_message>
small updates to cleaning
</commit_message>
<xml_diff>
--- a/Data/D2. CS/2016, 2017, 2018 & 2019- D2.8.SVY.BIZZ - REV.xlsx
+++ b/Data/D2. CS/2016, 2017, 2018 & 2019- D2.8.SVY.BIZZ - REV.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Aiesh\SPI 2019\SPI final files Dimensions 2 &amp; 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb469649\Documents\Github\SPI_AKI\Data\D2. CS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2C07A1-100A-4977-AA6F-185522F7FAD8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11519F51-2E2E-47A3-999E-826BFC263CC1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B1D4A2B0-B996-4285-8899-E61063B05042}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B1D4A2B0-B996-4285-8899-E61063B05042}"/>
   </bookViews>
   <sheets>
     <sheet name="2019 DCS" sheetId="13" r:id="rId1"/>
@@ -3580,7 +3580,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3710,6 +3710,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4041,17 +4044,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" style="55" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="55" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="55" customWidth="1"/>
-    <col min="4" max="5" width="9.5546875" style="55" customWidth="1"/>
-    <col min="6" max="27" width="8.88671875" style="48"/>
-    <col min="28" max="28" width="8.88671875" style="35"/>
+    <col min="2" max="2" width="13.54296875" style="55" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" style="55" customWidth="1"/>
+    <col min="4" max="5" width="9.54296875" style="55" customWidth="1"/>
+    <col min="6" max="27" width="8.90625" style="48"/>
+    <col min="28" max="28" width="8.90625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="44"/>
       <c r="B1" s="44"/>
       <c r="C1" s="44" t="s">
@@ -4130,7 +4133,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="44" t="s">
         <v>20</v>
       </c>
@@ -4165,7 +4168,7 @@
       <c r="Z2" s="44"/>
       <c r="AA2" s="44"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" s="45" t="s">
         <v>23</v>
       </c>
@@ -4249,7 +4252,7 @@
       </c>
       <c r="AB3"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
@@ -4333,7 +4336,7 @@
       </c>
       <c r="AB4"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" s="45" t="s">
         <v>25</v>
       </c>
@@ -4417,7 +4420,7 @@
       </c>
       <c r="AB5"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" s="49" t="s">
         <v>26</v>
       </c>
@@ -4501,7 +4504,7 @@
       </c>
       <c r="AB6"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" s="49" t="s">
         <v>27</v>
       </c>
@@ -4585,7 +4588,7 @@
       </c>
       <c r="AB7"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" s="45" t="s">
         <v>28</v>
       </c>
@@ -4669,7 +4672,7 @@
       </c>
       <c r="AB8"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" s="45" t="s">
         <v>29</v>
       </c>
@@ -4753,7 +4756,7 @@
       </c>
       <c r="AB9"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" s="45" t="s">
         <v>30</v>
       </c>
@@ -4837,7 +4840,7 @@
       </c>
       <c r="AB10"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" s="45" t="s">
         <v>31</v>
       </c>
@@ -4921,7 +4924,7 @@
       </c>
       <c r="AB11"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" s="49" t="s">
         <v>32</v>
       </c>
@@ -5005,7 +5008,7 @@
       </c>
       <c r="AB12"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" s="45" t="s">
         <v>33</v>
       </c>
@@ -5089,7 +5092,7 @@
       </c>
       <c r="AB13"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" s="45" t="s">
         <v>34</v>
       </c>
@@ -5173,7 +5176,7 @@
       </c>
       <c r="AB14"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" s="45" t="s">
         <v>35</v>
       </c>
@@ -5257,7 +5260,7 @@
       </c>
       <c r="AB15"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" s="45" t="s">
         <v>36</v>
       </c>
@@ -5341,7 +5344,7 @@
       </c>
       <c r="AB16"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A17" s="45" t="s">
         <v>37</v>
       </c>
@@ -5425,7 +5428,7 @@
       </c>
       <c r="AB17"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A18" s="49" t="s">
         <v>38</v>
       </c>
@@ -5509,7 +5512,7 @@
       </c>
       <c r="AB18"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A19" s="45" t="s">
         <v>39</v>
       </c>
@@ -5593,7 +5596,7 @@
       </c>
       <c r="AB19"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A20" s="45" t="s">
         <v>40</v>
       </c>
@@ -5677,7 +5680,7 @@
       </c>
       <c r="AB20"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A21" s="45" t="s">
         <v>41</v>
       </c>
@@ -5761,7 +5764,7 @@
       </c>
       <c r="AB21"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A22" s="45" t="s">
         <v>42</v>
       </c>
@@ -5845,7 +5848,7 @@
       </c>
       <c r="AB22"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A23" s="49" t="s">
         <v>43</v>
       </c>
@@ -5929,7 +5932,7 @@
       </c>
       <c r="AB23"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A24" s="45" t="s">
         <v>44</v>
       </c>
@@ -6013,7 +6016,7 @@
       </c>
       <c r="AB24"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A25" s="45" t="s">
         <v>45</v>
       </c>
@@ -6097,7 +6100,7 @@
       </c>
       <c r="AB25"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A26" s="45" t="s">
         <v>46</v>
       </c>
@@ -6181,7 +6184,7 @@
       </c>
       <c r="AB26"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A27" s="45" t="s">
         <v>47</v>
       </c>
@@ -6265,7 +6268,7 @@
       </c>
       <c r="AB27"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A28" s="49" t="s">
         <v>48</v>
       </c>
@@ -6349,7 +6352,7 @@
       </c>
       <c r="AB28"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A29" s="50" t="s">
         <v>49</v>
       </c>
@@ -6433,7 +6436,7 @@
       </c>
       <c r="AB29"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A30" s="49" t="s">
         <v>50</v>
       </c>
@@ -6517,7 +6520,7 @@
       </c>
       <c r="AB30"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A31" s="49" t="s">
         <v>51</v>
       </c>
@@ -6601,7 +6604,7 @@
       </c>
       <c r="AB31"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A32" s="45" t="s">
         <v>52</v>
       </c>
@@ -6685,7 +6688,7 @@
       </c>
       <c r="AB32"/>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A33" s="45" t="s">
         <v>53</v>
       </c>
@@ -6769,7 +6772,7 @@
       </c>
       <c r="AB33"/>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A34" s="49" t="s">
         <v>54</v>
       </c>
@@ -6853,7 +6856,7 @@
       </c>
       <c r="AB34"/>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A35" s="45" t="s">
         <v>55</v>
       </c>
@@ -6937,7 +6940,7 @@
       </c>
       <c r="AB35"/>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A36" s="45" t="s">
         <v>56</v>
       </c>
@@ -7021,7 +7024,7 @@
       </c>
       <c r="AB36"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A37" s="52" t="s">
         <v>57</v>
       </c>
@@ -7105,7 +7108,7 @@
       </c>
       <c r="AB37"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A38" s="45" t="s">
         <v>58</v>
       </c>
@@ -7189,7 +7192,7 @@
       </c>
       <c r="AB38"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A39" s="45" t="s">
         <v>59</v>
       </c>
@@ -7273,7 +7276,7 @@
       </c>
       <c r="AB39"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A40" s="52" t="s">
         <v>60</v>
       </c>
@@ -7357,7 +7360,7 @@
       </c>
       <c r="AB40"/>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A41" s="45" t="s">
         <v>61</v>
       </c>
@@ -7441,7 +7444,7 @@
       </c>
       <c r="AB41"/>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A42" s="45" t="s">
         <v>62</v>
       </c>
@@ -7525,7 +7528,7 @@
       </c>
       <c r="AB42"/>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A43" s="45" t="s">
         <v>63</v>
       </c>
@@ -7609,7 +7612,7 @@
       </c>
       <c r="AB43"/>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A44" s="45" t="s">
         <v>64</v>
       </c>
@@ -7693,7 +7696,7 @@
       </c>
       <c r="AB44"/>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A45" s="45" t="s">
         <v>65</v>
       </c>
@@ -7777,7 +7780,7 @@
       </c>
       <c r="AB45"/>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A46" s="49" t="s">
         <v>66</v>
       </c>
@@ -7861,7 +7864,7 @@
       </c>
       <c r="AB46"/>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A47" s="45" t="s">
         <v>67</v>
       </c>
@@ -7945,7 +7948,7 @@
       </c>
       <c r="AB47"/>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A48" s="45" t="s">
         <v>68</v>
       </c>
@@ -8029,7 +8032,7 @@
       </c>
       <c r="AB48"/>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A49" s="45" t="s">
         <v>69</v>
       </c>
@@ -8113,7 +8116,7 @@
       </c>
       <c r="AB49"/>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A50" s="45" t="s">
         <v>70</v>
       </c>
@@ -8197,7 +8200,7 @@
       </c>
       <c r="AB50"/>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A51" s="45" t="s">
         <v>71</v>
       </c>
@@ -8281,7 +8284,7 @@
       </c>
       <c r="AB51"/>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A52" s="52" t="s">
         <v>72</v>
       </c>
@@ -8365,7 +8368,7 @@
       </c>
       <c r="AB52"/>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A53" s="45" t="s">
         <v>73</v>
       </c>
@@ -8449,7 +8452,7 @@
       </c>
       <c r="AB53"/>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A54" s="45" t="s">
         <v>74</v>
       </c>
@@ -8533,7 +8536,7 @@
       </c>
       <c r="AB54"/>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A55" s="45" t="s">
         <v>75</v>
       </c>
@@ -8617,7 +8620,7 @@
       </c>
       <c r="AB55"/>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A56" s="45" t="s">
         <v>76</v>
       </c>
@@ -8701,7 +8704,7 @@
       </c>
       <c r="AB56"/>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A57" s="45" t="s">
         <v>77</v>
       </c>
@@ -8785,7 +8788,7 @@
       </c>
       <c r="AB57"/>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A58" s="45" t="s">
         <v>78</v>
       </c>
@@ -8869,7 +8872,7 @@
       </c>
       <c r="AB58"/>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A59" s="49" t="s">
         <v>79</v>
       </c>
@@ -8953,7 +8956,7 @@
       </c>
       <c r="AB59"/>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A60" s="45" t="s">
         <v>80</v>
       </c>
@@ -9037,7 +9040,7 @@
       </c>
       <c r="AB60"/>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A61" s="49" t="s">
         <v>81</v>
       </c>
@@ -9121,7 +9124,7 @@
       </c>
       <c r="AB61"/>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A62" s="45" t="s">
         <v>82</v>
       </c>
@@ -9205,7 +9208,7 @@
       </c>
       <c r="AB62"/>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A63" s="45" t="s">
         <v>83</v>
       </c>
@@ -9289,7 +9292,7 @@
       </c>
       <c r="AB63"/>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A64" s="45" t="s">
         <v>84</v>
       </c>
@@ -9373,7 +9376,7 @@
       </c>
       <c r="AB64"/>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A65" s="45" t="s">
         <v>85</v>
       </c>
@@ -9457,7 +9460,7 @@
       </c>
       <c r="AB65"/>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A66" s="45" t="s">
         <v>86</v>
       </c>
@@ -9541,7 +9544,7 @@
       </c>
       <c r="AB66"/>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A67" s="45" t="s">
         <v>87</v>
       </c>
@@ -9625,7 +9628,7 @@
       </c>
       <c r="AB67"/>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A68" s="45" t="s">
         <v>88</v>
       </c>
@@ -9709,7 +9712,7 @@
       </c>
       <c r="AB68"/>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A69" s="45" t="s">
         <v>89</v>
       </c>
@@ -9793,7 +9796,7 @@
       </c>
       <c r="AB69"/>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A70" s="52" t="s">
         <v>90</v>
       </c>
@@ -9877,7 +9880,7 @@
       </c>
       <c r="AB70"/>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A71" s="49" t="s">
         <v>91</v>
       </c>
@@ -9961,7 +9964,7 @@
       </c>
       <c r="AB71"/>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A72" s="45" t="s">
         <v>92</v>
       </c>
@@ -10045,7 +10048,7 @@
       </c>
       <c r="AB72"/>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A73" s="45" t="s">
         <v>93</v>
       </c>
@@ -10129,7 +10132,7 @@
       </c>
       <c r="AB73"/>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A74" s="45" t="s">
         <v>94</v>
       </c>
@@ -10213,7 +10216,7 @@
       </c>
       <c r="AB74"/>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A75" s="49" t="s">
         <v>117</v>
       </c>
@@ -10297,7 +10300,7 @@
       </c>
       <c r="AB75"/>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A76" s="45" t="s">
         <v>95</v>
       </c>
@@ -10381,7 +10384,7 @@
       </c>
       <c r="AB76"/>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A77" s="52" t="s">
         <v>96</v>
       </c>
@@ -10465,7 +10468,7 @@
       </c>
       <c r="AB77"/>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A78" s="45" t="s">
         <v>97</v>
       </c>
@@ -10549,7 +10552,7 @@
       </c>
       <c r="AB78"/>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A79" s="45" t="s">
         <v>98</v>
       </c>
@@ -10633,7 +10636,7 @@
       </c>
       <c r="AB79"/>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A80" s="45" t="s">
         <v>99</v>
       </c>
@@ -10717,7 +10720,7 @@
       </c>
       <c r="AB80"/>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A81" s="52" t="s">
         <v>100</v>
       </c>
@@ -10801,7 +10804,7 @@
       </c>
       <c r="AB81"/>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A82" s="49" t="s">
         <v>101</v>
       </c>
@@ -10885,7 +10888,7 @@
       </c>
       <c r="AB82"/>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A83" s="45" t="s">
         <v>102</v>
       </c>
@@ -10969,7 +10972,7 @@
       </c>
       <c r="AB83"/>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A84" s="45" t="s">
         <v>103</v>
       </c>
@@ -11053,7 +11056,7 @@
       </c>
       <c r="AB84"/>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A85" s="45" t="s">
         <v>104</v>
       </c>
@@ -11137,7 +11140,7 @@
       </c>
       <c r="AB85"/>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A86" s="45" t="s">
         <v>105</v>
       </c>
@@ -11221,7 +11224,7 @@
       </c>
       <c r="AB86"/>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A87" s="45" t="s">
         <v>106</v>
       </c>
@@ -11305,7 +11308,7 @@
       </c>
       <c r="AB87"/>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A88" s="45" t="s">
         <v>107</v>
       </c>
@@ -11389,7 +11392,7 @@
       </c>
       <c r="AB88"/>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A89" s="49" t="s">
         <v>108</v>
       </c>
@@ -11473,7 +11476,7 @@
       </c>
       <c r="AB89"/>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A90" s="45" t="s">
         <v>109</v>
       </c>
@@ -11557,7 +11560,7 @@
       </c>
       <c r="AB90"/>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A91" s="45" t="s">
         <v>110</v>
       </c>
@@ -11641,7 +11644,7 @@
       </c>
       <c r="AB91"/>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A92" s="45" t="s">
         <v>111</v>
       </c>
@@ -11725,7 +11728,7 @@
       </c>
       <c r="AB92"/>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A93" s="45" t="s">
         <v>112</v>
       </c>
@@ -11809,7 +11812,7 @@
       </c>
       <c r="AB93"/>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A94" s="45" t="s">
         <v>113</v>
       </c>
@@ -11893,7 +11896,7 @@
       </c>
       <c r="AB94"/>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A95" s="45" t="s">
         <v>114</v>
       </c>
@@ -11977,7 +11980,7 @@
       </c>
       <c r="AB95"/>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A96" s="45" t="s">
         <v>115</v>
       </c>
@@ -12061,7 +12064,7 @@
       </c>
       <c r="AB96"/>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A97" s="45" t="s">
         <v>116</v>
       </c>
@@ -12145,7 +12148,7 @@
       </c>
       <c r="AB97"/>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A98" s="45" t="s">
         <v>118</v>
       </c>
@@ -12229,7 +12232,7 @@
       </c>
       <c r="AB98"/>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A99" s="45" t="s">
         <v>119</v>
       </c>
@@ -12313,7 +12316,7 @@
       </c>
       <c r="AB99"/>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A100" s="45" t="s">
         <v>120</v>
       </c>
@@ -12397,7 +12400,7 @@
       </c>
       <c r="AB100"/>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A101" s="49" t="s">
         <v>121</v>
       </c>
@@ -12481,7 +12484,7 @@
       </c>
       <c r="AB101"/>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A102" s="45" t="s">
         <v>122</v>
       </c>
@@ -12565,7 +12568,7 @@
       </c>
       <c r="AB102"/>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A103" s="45" t="s">
         <v>123</v>
       </c>
@@ -12649,7 +12652,7 @@
       </c>
       <c r="AB103"/>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A104" s="45" t="s">
         <v>124</v>
       </c>
@@ -12733,7 +12736,7 @@
       </c>
       <c r="AB104"/>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A105" s="45" t="s">
         <v>125</v>
       </c>
@@ -12817,7 +12820,7 @@
       </c>
       <c r="AB105"/>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A106" s="49" t="s">
         <v>126</v>
       </c>
@@ -12901,7 +12904,7 @@
       </c>
       <c r="AB106"/>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A107" s="45" t="s">
         <v>127</v>
       </c>
@@ -12985,7 +12988,7 @@
       </c>
       <c r="AB107"/>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A108" s="45" t="s">
         <v>128</v>
       </c>
@@ -13069,7 +13072,7 @@
       </c>
       <c r="AB108"/>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A109" s="45" t="s">
         <v>129</v>
       </c>
@@ -13153,7 +13156,7 @@
       </c>
       <c r="AB109"/>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A110" s="45" t="s">
         <v>130</v>
       </c>
@@ -13237,7 +13240,7 @@
       </c>
       <c r="AB110"/>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A111" s="45" t="s">
         <v>131</v>
       </c>
@@ -13321,7 +13324,7 @@
       </c>
       <c r="AB111"/>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A112" s="49" t="s">
         <v>132</v>
       </c>
@@ -13405,7 +13408,7 @@
       </c>
       <c r="AB112"/>
     </row>
-    <row r="113" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A113" s="45" t="s">
         <v>133</v>
       </c>
@@ -13489,7 +13492,7 @@
       </c>
       <c r="AB113"/>
     </row>
-    <row r="114" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A114" s="49" t="s">
         <v>134</v>
       </c>
@@ -13573,7 +13576,7 @@
       </c>
       <c r="AB114"/>
     </row>
-    <row r="115" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A115" s="52" t="s">
         <v>135</v>
       </c>
@@ -13657,7 +13660,7 @@
       </c>
       <c r="AB115"/>
     </row>
-    <row r="116" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A116" s="45" t="s">
         <v>136</v>
       </c>
@@ -13741,7 +13744,7 @@
       </c>
       <c r="AB116"/>
     </row>
-    <row r="117" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A117" s="45" t="s">
         <v>137</v>
       </c>
@@ -13825,7 +13828,7 @@
       </c>
       <c r="AB117"/>
     </row>
-    <row r="118" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A118" s="49" t="s">
         <v>138</v>
       </c>
@@ -13909,7 +13912,7 @@
       </c>
       <c r="AB118"/>
     </row>
-    <row r="119" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A119" s="45" t="s">
         <v>139</v>
       </c>
@@ -13993,7 +13996,7 @@
       </c>
       <c r="AB119"/>
     </row>
-    <row r="120" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A120" s="49" t="s">
         <v>140</v>
       </c>
@@ -14077,7 +14080,7 @@
       </c>
       <c r="AB120"/>
     </row>
-    <row r="121" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A121" s="49" t="s">
         <v>141</v>
       </c>
@@ -14161,7 +14164,7 @@
       </c>
       <c r="AB121"/>
     </row>
-    <row r="122" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A122" s="46" t="s">
         <v>142</v>
       </c>
@@ -14245,7 +14248,7 @@
       </c>
       <c r="AB122"/>
     </row>
-    <row r="123" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A123" s="45" t="s">
         <v>143</v>
       </c>
@@ -14329,7 +14332,7 @@
       </c>
       <c r="AB123"/>
     </row>
-    <row r="124" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A124" s="45" t="s">
         <v>144</v>
       </c>
@@ -14413,7 +14416,7 @@
       </c>
       <c r="AB124"/>
     </row>
-    <row r="125" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A125" s="49" t="s">
         <v>145</v>
       </c>
@@ -14497,7 +14500,7 @@
       </c>
       <c r="AB125"/>
     </row>
-    <row r="126" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A126" s="49" t="s">
         <v>146</v>
       </c>
@@ -14581,7 +14584,7 @@
       </c>
       <c r="AB126"/>
     </row>
-    <row r="127" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A127" s="49" t="s">
         <v>147</v>
       </c>
@@ -14665,7 +14668,7 @@
       </c>
       <c r="AB127"/>
     </row>
-    <row r="128" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A128" s="49" t="s">
         <v>148</v>
       </c>
@@ -14749,7 +14752,7 @@
       </c>
       <c r="AB128"/>
     </row>
-    <row r="129" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A129" s="49" t="s">
         <v>149</v>
       </c>
@@ -14833,7 +14836,7 @@
       </c>
       <c r="AB129"/>
     </row>
-    <row r="130" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A130" s="49" t="s">
         <v>150</v>
       </c>
@@ -14917,7 +14920,7 @@
       </c>
       <c r="AB130"/>
     </row>
-    <row r="131" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A131" s="49" t="s">
         <v>151</v>
       </c>
@@ -15001,7 +15004,7 @@
       </c>
       <c r="AB131"/>
     </row>
-    <row r="132" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A132" s="49" t="s">
         <v>152</v>
       </c>
@@ -15085,7 +15088,7 @@
       </c>
       <c r="AB132"/>
     </row>
-    <row r="133" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A133" s="45" t="s">
         <v>153</v>
       </c>
@@ -15169,7 +15172,7 @@
       </c>
       <c r="AB133"/>
     </row>
-    <row r="134" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A134" s="45" t="s">
         <v>154</v>
       </c>
@@ -15253,7 +15256,7 @@
       </c>
       <c r="AB134"/>
     </row>
-    <row r="135" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A135" s="49" t="s">
         <v>155</v>
       </c>
@@ -15337,7 +15340,7 @@
       </c>
       <c r="AB135"/>
     </row>
-    <row r="136" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A136" s="49" t="s">
         <v>156</v>
       </c>
@@ -15421,7 +15424,7 @@
       </c>
       <c r="AB136"/>
     </row>
-    <row r="137" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A137" s="49" t="s">
         <v>157</v>
       </c>
@@ -15505,7 +15508,7 @@
       </c>
       <c r="AB137"/>
     </row>
-    <row r="138" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A138" s="49" t="s">
         <v>158</v>
       </c>
@@ -15589,7 +15592,7 @@
       </c>
       <c r="AB138"/>
     </row>
-    <row r="139" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A139" s="54" t="s">
         <v>159</v>
       </c>
@@ -15673,7 +15676,7 @@
       </c>
       <c r="AB139"/>
     </row>
-    <row r="140" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A140" s="49" t="s">
         <v>160</v>
       </c>
@@ -15757,7 +15760,7 @@
       </c>
       <c r="AB140"/>
     </row>
-    <row r="141" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A141" s="54" t="s">
         <v>161</v>
       </c>
@@ -15841,7 +15844,7 @@
       </c>
       <c r="AB141"/>
     </row>
-    <row r="142" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A142" s="54" t="s">
         <v>162</v>
       </c>
@@ -15925,7 +15928,7 @@
       </c>
       <c r="AB142"/>
     </row>
-    <row r="143" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A143" s="54" t="s">
         <v>163</v>
       </c>
@@ -16009,7 +16012,7 @@
       </c>
       <c r="AB143"/>
     </row>
-    <row r="144" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A144" s="54" t="s">
         <v>164</v>
       </c>
@@ -16093,7 +16096,7 @@
       </c>
       <c r="AB144"/>
     </row>
-    <row r="145" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A145" s="54" t="s">
         <v>165</v>
       </c>
@@ -16177,7 +16180,7 @@
       </c>
       <c r="AB145"/>
     </row>
-    <row r="146" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A146" s="54" t="s">
         <v>166</v>
       </c>
@@ -16261,7 +16264,7 @@
       </c>
       <c r="AB146"/>
     </row>
-    <row r="147" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A147" s="55" t="s">
         <v>314</v>
       </c>
@@ -16348,6 +16351,7 @@
   </sheetData>
   <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16356,24 +16360,24 @@
   <dimension ref="A1:CC148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="G112" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="R159" sqref="R159"/>
+      <selection pane="bottomRight" activeCell="I151" sqref="I151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="4.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.5546875" style="3" customWidth="1"/>
-    <col min="7" max="28" width="8.88671875" style="24"/>
-    <col min="29" max="16384" width="8.88671875" style="25"/>
+    <col min="1" max="2" width="4.08984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.54296875" style="3" customWidth="1"/>
+    <col min="7" max="28" width="8.90625" style="24"/>
+    <col min="29" max="16384" width="8.90625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="E1" s="12" t="s">
         <v>319</v>
       </c>
@@ -16384,7 +16388,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="C2" s="2">
         <v>1</v>
       </c>
@@ -16465,7 +16469,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>167</v>
       </c>
@@ -16552,7 +16556,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -16642,7 +16646,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <f t="shared" ref="A5:A10" si="0">1+A4</f>
         <v>2</v>
@@ -16733,7 +16737,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -16824,7 +16828,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -16915,7 +16919,7 @@
         <v xml:space="preserve">2006, 2010, </v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -17006,7 +17010,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -17097,7 +17101,7 @@
         <v xml:space="preserve">2010, </v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17188,7 +17192,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -17279,7 +17283,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -17370,7 +17374,7 @@
         <v xml:space="preserve">2010, </v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -17461,7 +17465,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -17552,7 +17556,7 @@
         <v xml:space="preserve">2016, </v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="e">
         <f t="shared" ref="A15:A20" si="2">1+A14</f>
         <v>#REF!</v>
@@ -17643,7 +17647,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="e">
         <f t="shared" si="2"/>
         <v>#REF!</v>
@@ -17734,7 +17738,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="e">
         <f t="shared" si="2"/>
         <v>#REF!</v>
@@ -17825,7 +17829,7 @@
         <v xml:space="preserve">2004, </v>
       </c>
     </row>
-    <row r="18" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="e">
         <f t="shared" si="2"/>
         <v>#REF!</v>
@@ -17916,7 +17920,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="e">
         <f t="shared" si="2"/>
         <v>#REF!</v>
@@ -18007,7 +18011,7 @@
         <v xml:space="preserve">2006, 2010, </v>
       </c>
     </row>
-    <row r="20" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="e">
         <f t="shared" si="2"/>
         <v>#REF!</v>
@@ -18098,7 +18102,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:81" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:81" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -18215,7 +18219,7 @@
       <c r="BB21" s="24"/>
       <c r="BC21" s="24"/>
     </row>
-    <row r="22" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="e">
         <f>1+A21</f>
         <v>#REF!</v>
@@ -18306,7 +18310,7 @@
         <v xml:space="preserve">2009, </v>
       </c>
     </row>
-    <row r="23" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="e">
         <f>1+A22</f>
         <v>#REF!</v>
@@ -18397,7 +18401,7 @@
         <v xml:space="preserve">2005, </v>
       </c>
     </row>
-    <row r="24" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="e">
         <f>1+A23</f>
         <v>#REF!</v>
@@ -18488,7 +18492,7 @@
         <v xml:space="preserve">2009, </v>
       </c>
     </row>
-    <row r="25" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="e">
         <f>1+A24</f>
         <v>#REF!</v>
@@ -18579,7 +18583,7 @@
         <v xml:space="preserve">1999, 2005, 2008, 2009, 2010, 2013, 2016, </v>
       </c>
     </row>
-    <row r="26" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="e">
         <f>1+A25</f>
         <v>#REF!</v>
@@ -18670,7 +18674,7 @@
         <v xml:space="preserve">2006, 2009, 2017, </v>
       </c>
     </row>
-    <row r="27" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -18813,7 +18817,7 @@
       <c r="CB27" s="35"/>
       <c r="CC27" s="35"/>
     </row>
-    <row r="28" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="e">
         <f t="shared" ref="A28:A37" si="3">1+A27</f>
         <v>#REF!</v>
@@ -18904,7 +18908,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:81" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:81" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="e">
         <f t="shared" si="3"/>
         <v>#REF!</v>
@@ -19047,7 +19051,7 @@
       <c r="CB29" s="35"/>
       <c r="CC29" s="35"/>
     </row>
-    <row r="30" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="e">
         <f t="shared" si="3"/>
         <v>#REF!</v>
@@ -19138,7 +19142,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="e">
         <f t="shared" si="3"/>
         <v>#REF!</v>
@@ -19229,7 +19233,7 @@
         <v xml:space="preserve">2008, 2009, 2010, 2011, 2012, </v>
       </c>
     </row>
-    <row r="32" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="e">
         <f t="shared" si="3"/>
         <v>#REF!</v>
@@ -19320,7 +19324,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="e">
         <f t="shared" si="3"/>
         <v>#REF!</v>
@@ -19411,7 +19415,7 @@
         <v xml:space="preserve">2006, 2010, 2014, </v>
       </c>
     </row>
-    <row r="34" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="e">
         <f t="shared" si="3"/>
         <v>#REF!</v>
@@ -19502,7 +19506,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="e">
         <f t="shared" si="3"/>
         <v>#REF!</v>
@@ -19593,7 +19597,7 @@
         <v xml:space="preserve">2011, 2016, 2017, </v>
       </c>
     </row>
-    <row r="36" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="e">
         <f t="shared" si="3"/>
         <v>#REF!</v>
@@ -19684,7 +19688,7 @@
         <v xml:space="preserve">2009, 2017, </v>
       </c>
     </row>
-    <row r="37" spans="1:55" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:55" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="e">
         <f t="shared" si="3"/>
         <v>#REF!</v>
@@ -19801,7 +19805,7 @@
       <c r="BB37" s="24"/>
       <c r="BC37" s="24"/>
     </row>
-    <row r="38" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -19892,7 +19896,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="e">
         <f t="shared" ref="A39:A45" si="4">1+A38</f>
         <v>#REF!</v>
@@ -19983,7 +19987,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="e">
         <f t="shared" si="4"/>
         <v>#REF!</v>
@@ -20074,7 +20078,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="e">
         <f t="shared" si="4"/>
         <v>#REF!</v>
@@ -20165,7 +20169,7 @@
         <v xml:space="preserve">2006, 2007, 2008, 2009, 2010, 2012, 2013, 2014, 2015, </v>
       </c>
     </row>
-    <row r="42" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="e">
         <f t="shared" si="4"/>
         <v>#REF!</v>
@@ -20256,7 +20260,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="e">
         <f t="shared" si="4"/>
         <v>#REF!</v>
@@ -20347,7 +20351,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="e">
         <f t="shared" si="4"/>
         <v>#REF!</v>
@@ -20438,7 +20442,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="e">
         <f t="shared" si="4"/>
         <v>#REF!</v>
@@ -20529,7 +20533,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -20620,7 +20624,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="e">
         <f>1+A46</f>
         <v>#REF!</v>
@@ -20711,7 +20715,7 @@
         <v xml:space="preserve">1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, </v>
       </c>
     </row>
-    <row r="48" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="e">
         <f>1+A47</f>
         <v>#REF!</v>
@@ -20802,7 +20806,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -20893,7 +20897,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="e">
         <f>1+A49</f>
         <v>#REF!</v>
@@ -20984,7 +20988,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="e">
         <f>1+A50</f>
         <v>#REF!</v>
@@ -21075,7 +21079,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -21166,7 +21170,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -21257,7 +21261,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="e">
         <f t="shared" ref="A54:A59" si="5">1+A53</f>
         <v>#REF!</v>
@@ -21348,7 +21352,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="e">
         <f t="shared" si="5"/>
         <v>#REF!</v>
@@ -21439,7 +21443,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="e">
         <f t="shared" si="5"/>
         <v>#REF!</v>
@@ -21530,7 +21534,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="e">
         <f t="shared" si="5"/>
         <v>#REF!</v>
@@ -21621,7 +21625,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="e">
         <f t="shared" si="5"/>
         <v>#REF!</v>
@@ -21712,7 +21716,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="e">
         <f t="shared" si="5"/>
         <v>#REF!</v>
@@ -21803,7 +21807,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -21894,7 +21898,7 @@
         <v xml:space="preserve">1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, </v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="e">
         <f>1+A60</f>
         <v>#REF!</v>
@@ -21985,7 +21989,7 @@
         <v xml:space="preserve">1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, </v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="e">
         <f>1+A61</f>
         <v>#REF!</v>
@@ -22076,7 +22080,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="e">
         <f>1+A62</f>
         <v>#REF!</v>
@@ -22167,7 +22171,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -22258,7 +22262,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -22349,7 +22353,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="e">
         <f>1+A65</f>
         <v>#REF!</v>
@@ -22440,7 +22444,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="e">
         <f>1+A66</f>
         <v>#REF!</v>
@@ -22531,7 +22535,7 @@
         <v xml:space="preserve">1999, </v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="e">
         <f>1+A67</f>
         <v>#REF!</v>
@@ -22622,7 +22626,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -22713,7 +22717,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -22804,7 +22808,7 @@
         <v xml:space="preserve">2003, </v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="e">
         <f>1+A70</f>
         <v>#REF!</v>
@@ -22895,7 +22899,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -22986,7 +22990,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="e">
         <f>1+A72</f>
         <v>#REF!</v>
@@ -23077,7 +23081,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="e">
         <f>1+A73</f>
         <v>#REF!</v>
@@ -23168,7 +23172,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="e">
         <f>1+A74</f>
         <v>#REF!</v>
@@ -23259,7 +23263,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="14" t="e">
         <f>1+#REF!</f>
         <v>#REF!</v>
@@ -23350,7 +23354,7 @@
         <v xml:space="preserve">2002, 2005, 2009, 2013, </v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A77" s="17">
         <v>100</v>
       </c>
@@ -23439,7 +23443,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A78" s="17">
         <v>101</v>
       </c>
@@ -23528,7 +23532,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A79" s="17">
         <v>102</v>
       </c>
@@ -23617,7 +23621,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A80" s="17">
         <v>103</v>
       </c>
@@ -23706,7 +23710,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A81" s="17">
         <v>104</v>
       </c>
@@ -23795,7 +23799,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A82" s="17">
         <v>106</v>
       </c>
@@ -23884,7 +23888,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A83" s="17">
         <v>107</v>
       </c>
@@ -23973,7 +23977,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A84" s="17">
         <v>108</v>
       </c>
@@ -24062,7 +24066,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A85" s="17">
         <v>109</v>
       </c>
@@ -24151,7 +24155,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A86" s="17">
         <v>110</v>
       </c>
@@ -24240,7 +24244,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A87" s="17">
         <v>111</v>
       </c>
@@ -24329,7 +24333,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A88" s="17">
         <v>112</v>
       </c>
@@ -24418,7 +24422,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A89" s="17">
         <v>113</v>
       </c>
@@ -24507,7 +24511,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A90" s="17">
         <v>114</v>
       </c>
@@ -24596,7 +24600,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A91" s="17">
         <v>115</v>
       </c>
@@ -24685,7 +24689,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A92" s="17">
         <v>116</v>
       </c>
@@ -24774,7 +24778,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A93" s="17">
         <v>117</v>
       </c>
@@ -24863,7 +24867,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A94" s="17">
         <v>118</v>
       </c>
@@ -24952,7 +24956,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A95" s="17">
         <v>119</v>
       </c>
@@ -25041,7 +25045,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A96" s="17">
         <v>122</v>
       </c>
@@ -25130,7 +25134,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A97" s="17">
         <v>123</v>
       </c>
@@ -25219,7 +25223,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A98" s="17">
         <v>124</v>
       </c>
@@ -25308,7 +25312,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A99" s="17">
         <v>128</v>
       </c>
@@ -25397,7 +25401,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A100" s="17">
         <v>129</v>
       </c>
@@ -25486,7 +25490,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A101" s="17">
         <v>130</v>
       </c>
@@ -25575,7 +25579,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A102" s="17">
         <v>131</v>
       </c>
@@ -25664,7 +25668,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A103" s="17">
         <v>132</v>
       </c>
@@ -25753,7 +25757,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A104" s="17">
         <v>133</v>
       </c>
@@ -25842,7 +25846,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A105" s="17">
         <v>134</v>
       </c>
@@ -25931,7 +25935,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A106" s="17">
         <v>135</v>
       </c>
@@ -26020,7 +26024,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A107" s="17">
         <v>138</v>
       </c>
@@ -26109,7 +26113,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A108" s="17">
         <v>139</v>
       </c>
@@ -26198,7 +26202,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A109" s="17">
         <v>140</v>
       </c>
@@ -26287,7 +26291,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A110" s="17">
         <v>141</v>
       </c>
@@ -26376,7 +26380,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A111" s="17">
         <v>143</v>
       </c>
@@ -26465,7 +26469,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A112" s="17">
         <v>145</v>
       </c>
@@ -26554,7 +26558,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A113" s="17">
         <v>146</v>
       </c>
@@ -26643,7 +26647,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="114" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A114" s="17">
         <v>147</v>
       </c>
@@ -26732,7 +26736,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="115" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A115" s="17">
         <v>148</v>
       </c>
@@ -26821,7 +26825,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A116" s="17">
         <v>152</v>
       </c>
@@ -26910,7 +26914,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A117" s="17">
         <v>153</v>
       </c>
@@ -26999,7 +27003,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A118" s="17">
         <v>154</v>
       </c>
@@ -27088,7 +27092,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A119" s="17">
         <v>155</v>
       </c>
@@ -27177,7 +27181,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A120" s="17">
         <v>157</v>
       </c>
@@ -27266,7 +27270,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A121" s="17">
         <v>158</v>
       </c>
@@ -27355,7 +27359,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A122" s="17">
         <v>159</v>
       </c>
@@ -27444,7 +27448,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A123" s="17">
         <v>160</v>
       </c>
@@ -27533,7 +27537,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A124" s="17">
         <v>161</v>
       </c>
@@ -27622,7 +27626,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A125" s="17">
         <v>162</v>
       </c>
@@ -27711,7 +27715,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A126" s="17">
         <v>165</v>
       </c>
@@ -27800,7 +27804,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A127" s="17">
         <v>166</v>
       </c>
@@ -27889,7 +27893,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A128" s="17">
         <v>167</v>
       </c>
@@ -27978,7 +27982,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A129" s="17">
         <v>168</v>
       </c>
@@ -28067,7 +28071,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A130" s="17">
         <v>169</v>
       </c>
@@ -28156,7 +28160,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A131" s="17">
         <v>170</v>
       </c>
@@ -28245,7 +28249,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A132" s="17">
         <v>171</v>
       </c>
@@ -28334,7 +28338,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A133" s="17">
         <v>172</v>
       </c>
@@ -28423,7 +28427,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A134" s="17">
         <v>173</v>
       </c>
@@ -28512,7 +28516,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A135" s="17">
         <v>174</v>
       </c>
@@ -28601,7 +28605,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A136" s="17">
         <v>175</v>
       </c>
@@ -28690,7 +28694,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A137" s="17">
         <v>176</v>
       </c>
@@ -28779,7 +28783,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A138" s="17">
         <v>177</v>
       </c>
@@ -28868,7 +28872,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A139" s="17">
         <v>178</v>
       </c>
@@ -28957,7 +28961,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A140" s="17">
         <v>182</v>
       </c>
@@ -29046,7 +29050,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="141" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A141" s="17">
         <v>183</v>
       </c>
@@ -29135,7 +29139,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="142" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A142" s="17">
         <v>184</v>
       </c>
@@ -29224,7 +29228,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="143" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A143" s="17">
         <v>185</v>
       </c>
@@ -29313,7 +29317,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="144" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A144" s="17">
         <v>186</v>
       </c>
@@ -29402,7 +29406,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="145" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A145" s="17">
         <v>187</v>
       </c>
@@ -29491,7 +29495,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="146" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A146" s="17">
         <v>188</v>
       </c>
@@ -29580,7 +29584,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="147" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A147" s="17">
         <v>189</v>
       </c>
@@ -29669,15 +29673,15 @@
         <v>322</v>
       </c>
     </row>
-    <row r="148" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A148" s="17">
         <v>190</v>
       </c>
       <c r="B148" s="5">
         <v>145</v>
       </c>
-      <c r="C148" s="18" t="s">
-        <v>309</v>
+      <c r="C148" s="56" t="s">
+        <v>314</v>
       </c>
       <c r="D148" s="23" t="s">
         <v>309</v>
@@ -29770,12 +29774,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29951,15 +29952,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8001F0D6-2591-4A68-815D-C98503A36C32}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACEEE91F-8CDF-4F2C-85D3-58EC881B6941}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="66105097-ee36-46f0-bac2-3eec24bcac6a"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -29983,17 +29995,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACEEE91F-8CDF-4F2C-85D3-58EC881B6941}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8001F0D6-2591-4A68-815D-C98503A36C32}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="66105097-ee36-46f0-bac2-3eec24bcac6a"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>